<commit_message>
aded defendant id back in
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="1180">
   <si>
     <t>Race</t>
   </si>
@@ -3554,6 +3554,15 @@
   </si>
   <si>
     <t xml:space="preserve">Person description ? Msj: person's role in the case - defendant, victim, witness? </t>
+  </si>
+  <si>
+    <t>Party ID</t>
+  </si>
+  <si>
+    <t>VW_PARTIES_CASES/PARTY_ID</t>
+  </si>
+  <si>
+    <t>unique identifier of a person</t>
   </si>
 </sst>
 </file>
@@ -4488,7 +4497,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4660,6 +4669,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5738,8 +5750,8 @@
   <dimension ref="A1:J309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D83" sqref="D83"/>
+      <pane ySplit="2" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7747,20 +7759,24 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
     </row>
-    <row r="100" spans="1:7" ht="28">
-      <c r="A100" s="37" t="s">
+    <row r="100" spans="1:7">
+      <c r="A100" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="B100" s="37" t="s">
-        <v>639</v>
-      </c>
-      <c r="C100" s="38" t="s">
-        <v>461</v>
-      </c>
+      <c r="B100" s="59" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C100" s="48"/>
       <c r="D100" s="48"/>
-      <c r="E100" s="55"/>
-      <c r="F100" s="55"/>
-      <c r="G100" s="55"/>
+      <c r="E100" s="55" t="s">
+        <v>565</v>
+      </c>
+      <c r="F100" s="55" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G100" s="55" t="s">
+        <v>1178</v>
+      </c>
     </row>
     <row r="101" spans="1:7" ht="28">
       <c r="A101" s="37" t="s">

</xml_diff>